<commit_message>
Cambios y correcciones generales
</commit_message>
<xml_diff>
--- a/src/nodes.xlsx
+++ b/src/nodes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="420" windowWidth="28515" windowHeight="12285" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="420" windowWidth="28515" windowHeight="12285" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="create-fields" sheetId="8" r:id="rId1"/>
@@ -12,12 +12,12 @@
     <sheet name="extras" sheetId="11" r:id="rId3"/>
     <sheet name="conditionals" sheetId="12" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="124">
   <si>
     <t>type</t>
   </si>
@@ -310,12 +310,6 @@
     <t>pending_payment</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>Fecha del pedido</t>
-  </si>
-  <si>
     <t>international-sale</t>
   </si>
   <si>
@@ -385,28 +379,16 @@
     <t>Precio de Venta (PV)</t>
   </si>
   <si>
-    <t>online_sale_items</t>
-  </si>
-  <si>
-    <t>international_sale_items</t>
-  </si>
-  <si>
-    <t>Fecha de envío</t>
-  </si>
-  <si>
-    <t>customer_email</t>
-  </si>
-  <si>
-    <t>customer_phone</t>
-  </si>
-  <si>
-    <t>total_price</t>
-  </si>
-  <si>
     <t>readonly</t>
   </si>
   <si>
     <t>print</t>
+  </si>
+  <si>
+    <t>sale-payment</t>
+  </si>
+  <si>
+    <t>sale-credit</t>
   </si>
 </sst>
 </file>
@@ -1079,10 +1061,10 @@
         <v>88</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>50</v>
@@ -1120,13 +1102,13 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>101</v>
-      </c>
       <c r="C8" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>50</v>
@@ -1228,10 +1210,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D97"/>
+  <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,7 +1277,7 @@
         <v>44</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1309,7 +1291,7 @@
         <v>44</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1323,7 +1305,7 @@
         <v>44</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1337,7 +1319,7 @@
         <v>44</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1351,7 +1333,7 @@
         <v>44</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1365,7 +1347,7 @@
         <v>44</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1379,7 +1361,7 @@
         <v>44</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1393,7 +1375,7 @@
         <v>44</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1407,7 +1389,7 @@
         <v>44</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1421,7 +1403,7 @@
         <v>44</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1435,7 +1417,7 @@
         <v>44</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1449,7 +1431,7 @@
         <v>44</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1463,12 +1445,12 @@
         <v>44</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>34</v>
@@ -1477,12 +1459,12 @@
         <v>44</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>34</v>
@@ -1491,7 +1473,7 @@
         <v>44</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1505,12 +1487,12 @@
         <v>44</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>34</v>
@@ -1519,12 +1501,12 @@
         <v>44</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>61</v>
@@ -1538,10 +1520,10 @@
     </row>
     <row r="22" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>44</v>
@@ -1552,10 +1534,10 @@
     </row>
     <row r="23" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>44</v>
@@ -1569,7 +1551,7 @@
         <v>92</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>44</v>
@@ -1583,7 +1565,7 @@
         <v>93</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>44</v>
@@ -1639,7 +1621,7 @@
         <v>90</v>
       </c>
       <c r="B29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>20</v>
@@ -1653,7 +1635,7 @@
         <v>90</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>44</v>
@@ -1863,13 +1845,13 @@
         <v>91</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1877,13 +1859,13 @@
         <v>91</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1939,7 +1921,7 @@
         <v>86</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1953,7 +1935,7 @@
         <v>86</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1967,7 +1949,7 @@
         <v>86</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2023,7 +2005,7 @@
         <v>86</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="57" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2037,7 +2019,7 @@
         <v>86</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2065,7 +2047,7 @@
         <v>86</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="60" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2241,7 +2223,7 @@
         <v>28</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>3</v>
@@ -2331,7 +2313,7 @@
         <v>86</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="79" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2345,7 +2327,7 @@
         <v>86</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="80" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2359,7 +2341,7 @@
         <v>86</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2376,228 +2358,32 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C82" s="4" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>122</v>
+      </c>
+      <c r="B82" t="s">
+        <v>60</v>
+      </c>
+      <c r="C82" t="s">
         <v>20</v>
       </c>
-      <c r="D82" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>88</v>
+        <v>123</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>125</v>
+        <v>38</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D84" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D85" s="4" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C86" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D86" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C87" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D87" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C88" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D88" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B89" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C89" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D89" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B90" t="s">
-        <v>122</v>
-      </c>
-      <c r="C90" t="s">
-        <v>15</v>
-      </c>
-      <c r="D90">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B91" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C91" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D91" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B92" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C92" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C93" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D93" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D94" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B95" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C95" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D95" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B96" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C96" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D96" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B97" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C97" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D97" s="4">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2608,10 +2394,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A45" sqref="A43:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2726,7 +2512,7 @@
         <v>28</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>66</v>
@@ -2768,7 +2554,7 @@
         <v>28</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>66</v>
@@ -2782,7 +2568,7 @@
         <v>28</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>66</v>
@@ -2796,7 +2582,7 @@
         <v>28</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>66</v>
@@ -2897,7 +2683,7 @@
         <v>70</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D20" s="5">
         <v>1</v>
@@ -2908,7 +2694,7 @@
         <v>28</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>84</v>
@@ -2922,7 +2708,7 @@
         <v>28</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>84</v>
@@ -2936,7 +2722,7 @@
         <v>28</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>84</v>
@@ -2950,7 +2736,7 @@
         <v>28</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>84</v>
@@ -3132,7 +2918,7 @@
         <v>56</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>39</v>
@@ -3146,7 +2932,7 @@
         <v>56</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>39</v>
@@ -3160,7 +2946,7 @@
         <v>76</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>39</v>
@@ -3211,87 +2997,31 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>81</v>
+    <row r="43" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="D43" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>82</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="D44" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D45" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D46" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D47" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D48" s="5">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correcciones en general y todotid
</commit_message>
<xml_diff>
--- a/src/nodes.xlsx
+++ b/src/nodes.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="127">
   <si>
     <t>type</t>
   </si>
@@ -389,6 +389,15 @@
   </si>
   <si>
     <t>sale-credit</t>
+  </si>
+  <si>
+    <t>cart</t>
+  </si>
+  <si>
+    <t>session_id</t>
+  </si>
+  <si>
+    <t>string</t>
   </si>
 </sst>
 </file>
@@ -1210,10 +1219,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D83"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C83" sqref="C83"/>
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2386,6 +2395,34 @@
         <v>32</v>
       </c>
     </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D84" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2396,7 +2433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A45" sqref="A43:XFD45"/>
     </sheetView>
   </sheetViews>

</xml_diff>